<commit_message>
Added powered by on signals
</commit_message>
<xml_diff>
--- a/public/assets/excelFiles/StockX_Headcount_2024.02.04.xlsx
+++ b/public/assets/excelFiles/StockX_Headcount_2024.02.04.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/howardzhong/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C28D69A-D1DC-1042-A89B-5D5E53484643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA25083C-BCFE-42D9-9456-9DB5B0334C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29920" yWindow="-840" windowWidth="38400" windowHeight="19980" xr2:uid="{5125CF4F-4348-4467-B0DA-444A74E4F9EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5125CF4F-4348-4467-B0DA-444A74E4F9EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -377,7 +377,7 @@
           <c:x val="1.7019339793372789E-2"/>
           <c:y val="6.0185185185185182E-2"/>
           <c:w val="0.96596132041325444"/>
-          <c:h val="0.76310950714494019"/>
+          <c:h val="0.67895548441206599"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -398,6 +398,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -406,22 +407,20 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
                         <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -861,16 +860,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -905,16 +904,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -958,7 +957,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="800">
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -993,9 +995,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="1.7019339793372789E-2"/>
-          <c:y val="6.0185185185185182E-2"/>
+          <c:y val="3.2407407407407406E-2"/>
           <c:w val="0.96596132041325444"/>
-          <c:h val="0.76310950714494019"/>
+          <c:h val="0.85107247010790321"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1016,6 +1018,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1024,22 +1027,20 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
                         <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -1246,20 +1247,20 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1295,16 +1296,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1348,7 +1349,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="800">
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1385,7 +1389,7 @@
           <c:x val="1.7019339793372789E-2"/>
           <c:y val="6.0185185185185182E-2"/>
           <c:w val="0.96596132041325444"/>
-          <c:h val="0.76310950714494019"/>
+          <c:h val="0.81858414488632436"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1406,6 +1410,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1414,22 +1419,20 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
                         <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -1464,23 +1467,23 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$85:$B$90</c:f>
+              <c:f>Sheet1!$B$86:$B$90</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2019</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>2019</c:v>
+                  <c:v>2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2020</c:v>
+                  <c:v>2021</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2021</c:v>
+                  <c:v>2022</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2022</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>2023</c:v>
                 </c:pt>
               </c:numCache>
@@ -1488,26 +1491,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$83:$C$90</c:f>
+              <c:f>Sheet1!$C$86:$C$90</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7901</c:v>
+                  <c:v>1557</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6382</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8079</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1557</c:v>
+                  <c:v>7112</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6382</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8079</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7112</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>7901</c:v>
                 </c:pt>
               </c:numCache>
@@ -1556,20 +1556,20 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1605,16 +1605,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1658,7 +1658,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="800">
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -3379,13 +3382,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>408214</xdr:colOff>
+      <xdr:colOff>408215</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>353785</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>403413</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>125026</xdr:rowOff>
     </xdr:to>
@@ -3716,20 +3719,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F14198B-0AA3-46E4-AF6C-4FAE93552632}">
   <dimension ref="B2:D90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A56" zoomScale="170" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.6640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="1"/>
-    <col min="2" max="2" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" style="2" customWidth="1"/>
-    <col min="5" max="74" width="6.6640625" style="1" customWidth="1"/>
-    <col min="75" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="6.7109375" style="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" style="2" customWidth="1"/>
+    <col min="5" max="74" width="6.7109375" style="1" customWidth="1"/>
+    <col min="75" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -3740,7 +3743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="4">
         <v>43496</v>
       </c>
@@ -3749,7 +3752,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="4">
         <v>43524</v>
       </c>
@@ -3758,7 +3761,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="4">
         <v>43555</v>
       </c>
@@ -3767,13 +3770,13 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="4">
         <v>43585</v>
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="4">
         <v>43616</v>
       </c>
@@ -3782,7 +3785,7 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="4">
         <v>43646</v>
       </c>
@@ -3791,7 +3794,7 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="4">
         <v>43677</v>
       </c>
@@ -3800,7 +3803,7 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="4">
         <v>43708</v>
       </c>
@@ -3809,13 +3812,13 @@
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="4">
         <v>43738</v>
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="4">
         <v>43769</v>
       </c>
@@ -3824,7 +3827,7 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="4">
         <v>43799</v>
       </c>
@@ -3833,7 +3836,7 @@
       </c>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="4">
         <v>43830</v>
       </c>
@@ -3842,7 +3845,7 @@
       </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" s="4">
         <v>43861</v>
       </c>
@@ -3854,7 +3857,7 @@
         <v>0.10486111111111107</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="4">
         <v>43890</v>
       </c>
@@ -3866,7 +3869,7 @@
         <v>9.3599449415003422E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="4">
         <v>43921</v>
       </c>
@@ -3878,7 +3881,7 @@
         <v>0.10808973487423512</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="4">
         <v>43951</v>
       </c>
@@ -3887,7 +3890,7 @@
       </c>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="4">
         <v>43982</v>
       </c>
@@ -3899,7 +3902,7 @@
         <v>5.1745635910224408E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="4">
         <v>44012</v>
       </c>
@@ -3911,7 +3914,7 @@
         <v>5.4020871700429796E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="4">
         <v>44043</v>
       </c>
@@ -3920,7 +3923,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="4">
         <v>44074</v>
       </c>
@@ -3932,7 +3935,7 @@
         <v>2.6814988290398127</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="4">
         <v>44104</v>
       </c>
@@ -3941,7 +3944,7 @@
       </c>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="4">
         <v>44135</v>
       </c>
@@ -3949,11 +3952,11 @@
         <v>6302</v>
       </c>
       <c r="D24" s="5">
-        <f>C24/C12-1</f>
+        <f t="shared" ref="D24:D32" si="0">C24/C12-1</f>
         <v>2.5990862364363223</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="4">
         <v>44165</v>
       </c>
@@ -3961,11 +3964,11 @@
         <v>6324</v>
       </c>
       <c r="D25" s="5">
-        <f>C25/C13-1</f>
+        <f t="shared" si="0"/>
         <v>2.5369127516778525</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="4">
         <v>44196</v>
       </c>
@@ -3973,11 +3976,11 @@
         <v>6382</v>
       </c>
       <c r="D26" s="5">
-        <f>C26/C14-1</f>
+        <f t="shared" si="0"/>
         <v>3.0989081567116248</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="4">
         <v>44227</v>
       </c>
@@ -3985,11 +3988,11 @@
         <v>6473</v>
       </c>
       <c r="D27" s="5">
-        <f>C27/C15-1</f>
+        <f t="shared" si="0"/>
         <v>3.068510370835952</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="4">
         <v>44255</v>
       </c>
@@ -3997,11 +4000,11 @@
         <v>6594</v>
       </c>
       <c r="D28" s="5">
-        <f>C28/C16-1</f>
+        <f t="shared" si="0"/>
         <v>3.1497797356828192</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="4">
         <v>44286</v>
       </c>
@@ -4009,11 +4012,11 @@
         <v>6648</v>
       </c>
       <c r="D29" s="5">
-        <f>C29/C17-1</f>
+        <f t="shared" si="0"/>
         <v>3.0785276073619636</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="4">
         <v>44316</v>
       </c>
@@ -4021,11 +4024,11 @@
         <v>6795</v>
       </c>
       <c r="D30" s="5">
-        <f>C30/C18-1</f>
+        <f t="shared" si="0"/>
         <v>3.1082224909310758</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="4">
         <v>44347</v>
       </c>
@@ -4033,11 +4036,11 @@
         <v>6896</v>
       </c>
       <c r="D31" s="5">
-        <f>C31/C19-1</f>
+        <f t="shared" si="0"/>
         <v>3.0877296976882036</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="4">
         <v>44377</v>
       </c>
@@ -4045,11 +4048,11 @@
         <v>7071</v>
       </c>
       <c r="D32" s="5">
-        <f>C32/C20-1</f>
+        <f t="shared" si="0"/>
         <v>3.118229470005824</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="4">
         <v>44408</v>
       </c>
@@ -4058,7 +4061,7 @@
       </c>
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="4">
         <v>44439</v>
       </c>
@@ -4066,11 +4069,11 @@
         <v>7620</v>
       </c>
       <c r="D34" s="5">
-        <f>C34/C22-1</f>
+        <f t="shared" ref="D34:D51" si="1">C34/C22-1</f>
         <v>0.21183206106870234</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="4">
         <v>44469</v>
       </c>
@@ -4078,11 +4081,11 @@
         <v>7773</v>
       </c>
       <c r="D35" s="5">
-        <f>C35/C23-1</f>
+        <f t="shared" si="1"/>
         <v>0.2397129186602871</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="4">
         <v>44500</v>
       </c>
@@ -4090,11 +4093,11 @@
         <v>7863</v>
       </c>
       <c r="D36" s="5">
-        <f>C36/C24-1</f>
+        <f t="shared" si="1"/>
         <v>0.2476991431291653</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="4">
         <v>44530</v>
       </c>
@@ -4102,11 +4105,11 @@
         <v>8148</v>
       </c>
       <c r="D37" s="5">
-        <f>C37/C25-1</f>
+        <f t="shared" si="1"/>
         <v>0.28842504743833008</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="4">
         <v>44561</v>
       </c>
@@ -4114,11 +4117,11 @@
         <v>8079</v>
       </c>
       <c r="D38" s="5">
-        <f>C38/C26-1</f>
+        <f t="shared" si="1"/>
         <v>0.2659041052961455</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="4">
         <v>44592</v>
       </c>
@@ -4126,20 +4129,20 @@
         <v>7985</v>
       </c>
       <c r="D39" s="5">
-        <f>C39/C27-1</f>
+        <f t="shared" si="1"/>
         <v>0.23358566352541321</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="4">
         <v>44620</v>
       </c>
       <c r="D40" s="5">
-        <f>C40/C28-1</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="4">
         <v>44651</v>
       </c>
@@ -4147,11 +4150,11 @@
         <v>7886</v>
       </c>
       <c r="D41" s="5">
-        <f>C41/C29-1</f>
+        <f t="shared" si="1"/>
         <v>0.18622141997593267</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="4">
         <v>44681</v>
       </c>
@@ -4159,11 +4162,11 @@
         <v>7598</v>
       </c>
       <c r="D42" s="5">
-        <f>C42/C30-1</f>
+        <f t="shared" si="1"/>
         <v>0.11817512877115521</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="4">
         <v>44712</v>
       </c>
@@ -4171,11 +4174,11 @@
         <v>7325</v>
       </c>
       <c r="D43" s="5">
-        <f>C43/C31-1</f>
+        <f t="shared" si="1"/>
         <v>6.2209976798143884E-2</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" s="4">
         <v>44742</v>
       </c>
@@ -4183,20 +4186,20 @@
         <v>7216</v>
       </c>
       <c r="D44" s="5">
-        <f>C44/C32-1</f>
+        <f t="shared" si="1"/>
         <v>2.0506293310705637E-2</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="4">
         <v>44773</v>
       </c>
       <c r="D45" s="5">
-        <f>C45/C33-1</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" s="4">
         <v>44804</v>
       </c>
@@ -4204,11 +4207,11 @@
         <v>7199</v>
       </c>
       <c r="D46" s="5">
-        <f>C46/C34-1</f>
+        <f t="shared" si="1"/>
         <v>-5.5249343832020958E-2</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="4">
         <v>44834</v>
       </c>
@@ -4216,11 +4219,11 @@
         <v>7102</v>
       </c>
       <c r="D47" s="5">
-        <f>C47/C35-1</f>
+        <f t="shared" si="1"/>
         <v>-8.6324456451820408E-2</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" s="4">
         <v>44865</v>
       </c>
@@ -4228,11 +4231,11 @@
         <v>7090</v>
       </c>
       <c r="D48" s="5">
-        <f>C48/C36-1</f>
+        <f t="shared" si="1"/>
         <v>-9.8308533638560291E-2</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="4">
         <v>44895</v>
       </c>
@@ -4240,11 +4243,11 @@
         <v>7086</v>
       </c>
       <c r="D49" s="5">
-        <f>C49/C37-1</f>
+        <f t="shared" si="1"/>
         <v>-0.13033873343151692</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="4">
         <v>44926</v>
       </c>
@@ -4252,11 +4255,11 @@
         <v>7112</v>
       </c>
       <c r="D50" s="5">
-        <f>C50/C38-1</f>
+        <f t="shared" si="1"/>
         <v>-0.11969303131575693</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" s="4">
         <v>44957</v>
       </c>
@@ -4264,11 +4267,11 @@
         <v>7107</v>
       </c>
       <c r="D51" s="5">
-        <f>C51/C39-1</f>
+        <f t="shared" si="1"/>
         <v>-0.10995616781465245</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" s="4">
         <v>44985</v>
       </c>
@@ -4277,7 +4280,7 @@
       </c>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" s="4">
         <v>45016</v>
       </c>
@@ -4289,7 +4292,7 @@
         <v>-9.332995181334014E-2</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" s="4">
         <v>45046</v>
       </c>
@@ -4301,7 +4304,7 @@
         <v>-6.3042906027902079E-2</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" s="4">
         <v>45077</v>
       </c>
@@ -4313,7 +4316,7 @@
         <v>-4.1774744027303745E-2</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" s="4">
         <v>45107</v>
       </c>
@@ -4325,7 +4328,7 @@
         <v>5.1136363636363535E-2</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" s="4">
         <v>45138</v>
       </c>
@@ -4334,7 +4337,7 @@
       </c>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" s="4">
         <v>45169</v>
       </c>
@@ -4346,7 +4349,7 @@
         <v>7.3760244478399795E-2</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" s="4">
         <v>45199</v>
       </c>
@@ -4358,7 +4361,7 @@
         <v>9.6874119966206651E-2</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" s="4">
         <v>45230</v>
       </c>
@@ -4370,7 +4373,7 @@
         <v>0.11763046544428768</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" s="4">
         <v>45260</v>
       </c>
@@ -4382,13 +4385,13 @@
         <v>0.11501552356759803</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62" s="4">
         <v>45291</v>
       </c>
       <c r="D62" s="5"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
         <v>2</v>
       </c>
@@ -4397,7 +4400,7 @@
       </c>
       <c r="D64" s="5"/>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
         <v>3</v>
       </c>
@@ -4406,7 +4409,7 @@
       </c>
       <c r="D65" s="5"/>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">
         <v>4</v>
       </c>
@@ -4417,7 +4420,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B67" s="2" t="s">
         <v>5</v>
       </c>
@@ -4428,7 +4431,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B68" s="2" t="s">
         <v>6</v>
       </c>
@@ -4440,7 +4443,7 @@
         <v>0.10808973487423512</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B69" s="2" t="s">
         <v>7</v>
       </c>
@@ -4448,11 +4451,11 @@
         <v>1717</v>
       </c>
       <c r="D69" s="5">
-        <f t="shared" ref="D69:D83" si="0">C69/C65-1</f>
+        <f t="shared" ref="D69:D83" si="2">C69/C65-1</f>
         <v>5.4020871700429796E-2</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B70" s="2" t="s">
         <v>8</v>
       </c>
@@ -4460,11 +4463,11 @@
         <v>6270</v>
       </c>
       <c r="D70" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.6709601873536299</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B71" s="2" t="s">
         <v>9</v>
       </c>
@@ -4472,11 +4475,11 @@
         <v>6382</v>
       </c>
       <c r="D71" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.0989081567116248</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B72" s="2" t="s">
         <v>10</v>
       </c>
@@ -4484,11 +4487,11 @@
         <v>6648</v>
       </c>
       <c r="D72" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.0785276073619636</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B73" s="2" t="s">
         <v>11</v>
       </c>
@@ -4496,11 +4499,11 @@
         <v>7071</v>
       </c>
       <c r="D73" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.118229470005824</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B74" s="2" t="s">
         <v>12</v>
       </c>
@@ -4508,11 +4511,11 @@
         <v>7773</v>
       </c>
       <c r="D74" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.2397129186602871</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B75" s="2" t="s">
         <v>13</v>
       </c>
@@ -4520,11 +4523,11 @@
         <v>8079</v>
       </c>
       <c r="D75" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.2659041052961455</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B76" s="2" t="s">
         <v>14</v>
       </c>
@@ -4532,11 +4535,11 @@
         <v>7886</v>
       </c>
       <c r="D76" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.18622141997593267</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B77" s="2" t="s">
         <v>15</v>
       </c>
@@ -4544,11 +4547,11 @@
         <v>7216</v>
       </c>
       <c r="D77" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0506293310705637E-2</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B78" s="2" t="s">
         <v>16</v>
       </c>
@@ -4556,11 +4559,11 @@
         <v>7102</v>
       </c>
       <c r="D78" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-8.6324456451820408E-2</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B79" s="2" t="s">
         <v>17</v>
       </c>
@@ -4568,11 +4571,11 @@
         <v>7112</v>
       </c>
       <c r="D79" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-0.11969303131575693</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B80" s="2" t="s">
         <v>18</v>
       </c>
@@ -4580,11 +4583,11 @@
         <v>7150</v>
       </c>
       <c r="D80" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-9.332995181334014E-2</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" s="2" t="s">
         <v>19</v>
       </c>
@@ -4592,11 +4595,11 @@
         <v>7585</v>
       </c>
       <c r="D81" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.1136363636363535E-2</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B82" s="2" t="s">
         <v>20</v>
       </c>
@@ -4604,11 +4607,11 @@
         <v>7790</v>
       </c>
       <c r="D82" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.6874119966206651E-2</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B83" s="2" t="s">
         <v>21</v>
       </c>
@@ -4616,11 +4619,11 @@
         <v>7901</v>
       </c>
       <c r="D83" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.11093925759280099</v>
       </c>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B86" s="2">
         <v>2019</v>
       </c>
@@ -4629,7 +4632,7 @@
       </c>
       <c r="D86" s="5"/>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B87" s="2">
         <v>2020</v>
       </c>
@@ -4640,7 +4643,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B88" s="2">
         <v>2021</v>
       </c>
@@ -4651,7 +4654,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B89" s="2">
         <v>2022</v>
       </c>
@@ -4662,7 +4665,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B90" s="2">
         <v>2023</v>
       </c>
@@ -4687,14 +4690,14 @@
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E22">
         <v>1415</v>
       </c>
     </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>0.98263888888888884</v>
       </c>
@@ -4702,7 +4705,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>23</v>
       </c>
@@ -4710,7 +4713,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>1.0777777777777777</v>
       </c>
@@ -4722,7 +4725,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1.1270833333333334</v>
       </c>
@@ -4730,7 +4733,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>1.1666666666666667</v>
       </c>
@@ -4738,7 +4741,7 @@
         <v>1453</v>
       </c>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>1.2173611111111111</v>
       </c>
@@ -4746,7 +4749,7 @@
         <v>1471</v>
       </c>
     </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>1.2715277777777778</v>
       </c>
@@ -4754,7 +4757,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>24</v>
       </c>
@@ -4762,7 +4765,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>1.4472222222222222</v>
       </c>
@@ -4770,7 +4773,7 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>1.5062499999999999</v>
       </c>
@@ -4781,7 +4784,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>1.5909722222222225</v>
       </c>
@@ -4789,7 +4792,7 @@
         <v>1708</v>
       </c>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>1.6444444444444446</v>
       </c>
@@ -4797,7 +4800,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>25</v>
       </c>
@@ -4805,7 +4808,7 @@
         <v>1751</v>
       </c>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>1.757638888888889</v>
       </c>
@@ -4813,7 +4816,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>1.825</v>
       </c>
@@ -4821,7 +4824,7 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>1.70625</v>
       </c>
@@ -4829,7 +4832,7 @@
         <v>1591</v>
       </c>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>1.7715277777777778</v>
       </c>
@@ -4837,7 +4840,7 @@
         <v>1589</v>
       </c>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>1.8118055555555557</v>
       </c>
@@ -4845,7 +4848,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>1.8819444444444446</v>
       </c>
@@ -4853,7 +4856,7 @@
         <v>1654</v>
       </c>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>1.9402777777777775</v>
       </c>
@@ -4861,7 +4864,7 @@
         <v>1687</v>
       </c>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>2.004861111111111</v>
       </c>
@@ -4869,7 +4872,7 @@
         <v>1717</v>
       </c>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>2.067361111111111</v>
       </c>
@@ -4877,7 +4880,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>26</v>
       </c>
@@ -4885,7 +4888,7 @@
         <v>6288</v>
       </c>
     </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>5.3250000000000002</v>
       </c>
@@ -4893,7 +4896,7 @@
         <v>6270</v>
       </c>
     </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>27</v>
       </c>
@@ -4901,7 +4904,7 @@
         <v>6302</v>
       </c>
     </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>28</v>
       </c>
@@ -4909,7 +4912,7 @@
         <v>6324</v>
       </c>
     </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>29</v>
       </c>
@@ -4917,7 +4920,7 @@
         <v>6382</v>
       </c>
     </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>30</v>
       </c>
@@ -4925,7 +4928,7 @@
         <v>6473</v>
       </c>
     </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>31</v>
       </c>
@@ -4933,7 +4936,7 @@
         <v>6594</v>
       </c>
     </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>32</v>
       </c>
@@ -4941,7 +4944,7 @@
         <v>6648</v>
       </c>
     </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
         <v>33</v>
       </c>
@@ -4949,7 +4952,7 @@
         <v>6795</v>
       </c>
     </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>34</v>
       </c>
@@ -4957,7 +4960,7 @@
         <v>6896</v>
       </c>
     </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>35</v>
       </c>
@@ -4965,7 +4968,7 @@
         <v>7071</v>
       </c>
     </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>36</v>
       </c>
@@ -4973,7 +4976,7 @@
         <v>7299</v>
       </c>
     </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>37</v>
       </c>
@@ -4981,7 +4984,7 @@
         <v>7620</v>
       </c>
     </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>38</v>
       </c>
@@ -4989,7 +4992,7 @@
         <v>7773</v>
       </c>
     </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>39</v>
       </c>
@@ -4997,7 +5000,7 @@
         <v>7863</v>
       </c>
     </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>40</v>
       </c>
@@ -5005,7 +5008,7 @@
         <v>8148</v>
       </c>
     </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>41</v>
       </c>
@@ -5013,7 +5016,7 @@
         <v>8079</v>
       </c>
     </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>42</v>
       </c>
@@ -5021,7 +5024,7 @@
         <v>7985</v>
       </c>
     </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>43</v>
       </c>
@@ -5029,7 +5032,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>44</v>
       </c>
@@ -5037,7 +5040,7 @@
         <v>7886</v>
       </c>
     </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>45</v>
       </c>
@@ -5045,7 +5048,7 @@
         <v>7598</v>
       </c>
     </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>46</v>
       </c>
@@ -5053,7 +5056,7 @@
         <v>7325</v>
       </c>
     </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>47</v>
       </c>
@@ -5061,7 +5064,7 @@
         <v>7216</v>
       </c>
     </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>48</v>
       </c>
@@ -5069,7 +5072,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>49</v>
       </c>
@@ -5077,7 +5080,7 @@
         <v>7199</v>
       </c>
     </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>50</v>
       </c>
@@ -5085,7 +5088,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>51</v>
       </c>
@@ -5093,7 +5096,7 @@
         <v>7090</v>
       </c>
     </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>52</v>
       </c>
@@ -5101,7 +5104,7 @@
         <v>7086</v>
       </c>
     </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
         <v>53</v>
       </c>
@@ -5109,7 +5112,7 @@
         <v>7112</v>
       </c>
     </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
         <v>54</v>
       </c>
@@ -5117,7 +5120,7 @@
         <v>7107</v>
       </c>
     </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>55</v>
       </c>
@@ -5125,7 +5128,7 @@
         <v>7112</v>
       </c>
     </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
         <v>56</v>
       </c>
@@ -5133,7 +5136,7 @@
         <v>7150</v>
       </c>
     </row>
-    <row r="77" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
         <v>57</v>
       </c>
@@ -5141,7 +5144,7 @@
         <v>7119</v>
       </c>
     </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>58</v>
       </c>
@@ -5149,7 +5152,7 @@
         <v>7019</v>
       </c>
     </row>
-    <row r="79" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
         <v>59</v>
       </c>
@@ -5157,7 +5160,7 @@
         <v>7585</v>
       </c>
     </row>
-    <row r="80" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
         <v>60</v>
       </c>
@@ -5165,7 +5168,7 @@
         <v>7670</v>
       </c>
     </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
         <v>61</v>
       </c>
@@ -5173,7 +5176,7 @@
         <v>7730</v>
       </c>
     </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
         <v>62</v>
       </c>
@@ -5181,7 +5184,7 @@
         <v>7790</v>
       </c>
     </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
         <v>63</v>
       </c>
@@ -5189,7 +5192,7 @@
         <v>7924</v>
       </c>
     </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>64</v>
       </c>
@@ -5197,7 +5200,7 @@
         <v>7901</v>
       </c>
     </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
         <v>65</v>
       </c>

</xml_diff>